<commit_message>
feat：fix world2 diamond num bug
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/SceneUnit_场景单位表.xlsx
+++ b/pet-simulator/Excel/SceneUnit_场景单位表.xlsx
@@ -1361,9 +1361,9 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="3" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L134" activeCellId="0" sqref="L134"/>
+      <selection pane="bottomLeft" activeCell="D114" activeCellId="0" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4713,7 +4713,7 @@
         <v>2002</v>
       </c>
       <c r="E71" s="33" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F71" s="34" t="n">
         <v>630000</v>
@@ -4759,7 +4759,7 @@
         <v>2002</v>
       </c>
       <c r="E72" s="37" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F72" s="34" t="n">
         <v>1512000</v>
@@ -4805,7 +4805,7 @@
         <v>2002</v>
       </c>
       <c r="E73" s="33" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F73" s="34" t="n">
         <v>157500</v>
@@ -5092,8 +5092,8 @@
       <c r="D79" s="17" t="n">
         <v>2004</v>
       </c>
-      <c r="E79" s="15" t="n">
-        <v>4</v>
+      <c r="E79" s="33" t="n">
+        <v>8</v>
       </c>
       <c r="F79" s="52" t="n">
         <v>1880000</v>
@@ -5137,8 +5137,8 @@
       <c r="D80" s="17" t="n">
         <v>2004</v>
       </c>
-      <c r="E80" s="21" t="n">
-        <v>2</v>
+      <c r="E80" s="37" t="n">
+        <v>4</v>
       </c>
       <c r="F80" s="16" t="n">
         <v>4500000</v>
@@ -5465,7 +5465,7 @@
         <v>2005</v>
       </c>
       <c r="E87" s="33" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F87" s="34" t="n">
         <v>4000000</v>
@@ -5510,7 +5510,7 @@
         <v>2005</v>
       </c>
       <c r="E88" s="37" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F88" s="34" t="n">
         <v>9600000</v>
@@ -5836,8 +5836,8 @@
       <c r="D95" s="17" t="n">
         <v>2006</v>
       </c>
-      <c r="E95" s="15" t="n">
-        <v>4</v>
+      <c r="E95" s="33" t="n">
+        <v>8</v>
       </c>
       <c r="F95" s="16" t="n">
         <v>8750000</v>
@@ -5881,8 +5881,8 @@
       <c r="D96" s="17" t="n">
         <v>2006</v>
       </c>
-      <c r="E96" s="21" t="n">
-        <v>2</v>
+      <c r="E96" s="37" t="n">
+        <v>4</v>
       </c>
       <c r="F96" s="16" t="n">
         <v>21000000</v>
@@ -6209,7 +6209,7 @@
         <v>2007</v>
       </c>
       <c r="E103" s="33" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F103" s="34" t="n">
         <v>20000000</v>
@@ -6254,7 +6254,7 @@
         <v>2007</v>
       </c>
       <c r="E104" s="37" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F104" s="34" t="n">
         <v>48000000</v>
@@ -6580,8 +6580,8 @@
       <c r="D111" s="17" t="n">
         <v>2008</v>
       </c>
-      <c r="E111" s="15" t="n">
-        <v>4</v>
+      <c r="E111" s="33" t="n">
+        <v>8</v>
       </c>
       <c r="F111" s="16" t="n">
         <v>45000000</v>
@@ -6625,8 +6625,8 @@
       <c r="D112" s="17" t="n">
         <v>2008</v>
       </c>
-      <c r="E112" s="21" t="n">
-        <v>2</v>
+      <c r="E112" s="37" t="n">
+        <v>4</v>
       </c>
       <c r="F112" s="16" t="n">
         <v>108000000</v>
@@ -6953,7 +6953,7 @@
         <v>2009</v>
       </c>
       <c r="E119" s="33" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F119" s="34" t="n">
         <v>62500000</v>
@@ -6998,7 +6998,7 @@
         <v>2009</v>
       </c>
       <c r="E120" s="37" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F120" s="34" t="n">
         <v>150000000</v>

</xml_diff>

<commit_message>
feat：update prefab bug fix
礼物箱失色问题处理
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/SceneUnit_场景单位表.xlsx
+++ b/pet-simulator/Excel/SceneUnit_场景单位表.xlsx
@@ -195,7 +195,7 @@
     <t xml:space="preserve">金币4</t>
   </si>
   <si>
-    <t xml:space="preserve">1FCF576C4A5031D9B3E87BA9D1C7A04A</t>
+    <t xml:space="preserve">C2C4639B48412430590BE1977AC37D35</t>
   </si>
   <si>
     <t xml:space="preserve">3|30</t>
@@ -1343,9 +1343,9 @@
   <dimension ref="A1:U131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
+      <selection pane="bottomLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat：fix coin box bug
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/SceneUnit_场景单位表.xlsx
+++ b/pet-simulator/Excel/SceneUnit_场景单位表.xlsx
@@ -195,7 +195,7 @@
     <t xml:space="preserve">金币4</t>
   </si>
   <si>
-    <t xml:space="preserve">1FCF576C4A5031D9B3E87BA9D1C7A04A</t>
+    <t xml:space="preserve">AF77EB51453E2ADC4DB5B3B7D4E8A349</t>
   </si>
   <si>
     <t xml:space="preserve">3|30</t>
@@ -1343,9 +1343,9 @@
   <dimension ref="A1:U131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
+      <selection pane="bottomLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>